<commit_message>
Add reference to calibration parameters
Add reference to calibration parameters for better understanding of the parameters
</commit_message>
<xml_diff>
--- a/excel_template.xlsx
+++ b/excel_template.xlsx
@@ -758,18 +758,6 @@
     <t>The fluorescence quantum yield of the acceptor</t>
   </si>
   <si>
-    <t>The alpha calibration parameter</t>
-  </si>
-  <si>
-    <t>The beta calibration parameter</t>
-  </si>
-  <si>
-    <t>The gamma calibration parameter</t>
-  </si>
-  <si>
-    <t>The delta calibration parameter</t>
-  </si>
-  <si>
     <t>The gG/gR ratio</t>
   </si>
   <si>
@@ -2042,9 +2030,6 @@
     <t>Sample ID</t>
   </si>
   <si>
-    <t>The fraction of bright molecules</t>
-  </si>
-  <si>
     <t>Journal abbreviation</t>
   </si>
   <si>
@@ -2553,6 +2538,21 @@
   </si>
   <si>
     <t>Template version 1.0</t>
+  </si>
+  <si>
+    <t>The alpha calibration parameter (cf. Hellenkamp et al. DOI: 10.1038/s41592-018-0085-0 )</t>
+  </si>
+  <si>
+    <t>The beta calibration parameter (cf. Hellenkamp et al. DOI: 10.1038/s41592-018-0085-0 )</t>
+  </si>
+  <si>
+    <t>The gamma calibration parameter (cf. Hellenkamp et al. DOI: 10.1038/s41592-018-0085-0 )</t>
+  </si>
+  <si>
+    <t>The delta calibration parameter (cf. Hellenkamp et al. DOI: 10.1038/s41592-018-0085-0 )</t>
+  </si>
+  <si>
+    <t>The fraction of bright molecules (cf. Hellenkamp et al. DOI: 10.1038/s41592-018-0085-0 )</t>
   </si>
 </sst>
 </file>
@@ -3072,19 +3072,19 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3100,7 +3100,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
     </row>
   </sheetData>
@@ -3168,121 +3168,121 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="22" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>776</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>705</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>777</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>778</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>706</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>707</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>708</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>709</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>781</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>710</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>782</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>783</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>711</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>712</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>713</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>715</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="B3" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C3" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="G3" t="s">
         <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="I3" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J3" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="K3" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="L3" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>555</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>556</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>557</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>563</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>562</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="J4" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>561</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>560</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>559</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>564</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>565</v>
-      </c>
       <c r="L4" s="9" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -3330,36 +3330,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="22" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>713</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>780</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>715</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>716</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>781</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>717</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>718</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>785</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>719</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>720</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>721</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>786</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -3393,31 +3393,31 @@
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="I4" s="9" t="s">
         <v>433</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>435</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>436</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -3445,42 +3445,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="22" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -3491,7 +3491,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -3515,42 +3515,42 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>424</v>
-      </c>
       <c r="K4" s="9" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3611,103 +3611,103 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>723</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>789</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>790</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>724</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>725</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>726</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>727</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>728</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>795</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>729</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>730</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>731</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>732</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>733</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="110.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>585</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>591</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>592</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>593</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>595</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -3736,8 +3736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DJ11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+    <sheetView topLeftCell="BL1" workbookViewId="0">
+      <selection activeCell="BS3" sqref="BS3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3764,7 +3764,7 @@
   <sheetData>
     <row r="1" spans="1:114" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="B1" s="26"/>
       <c r="E1" s="26"/>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="2" spans="1:114" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>147</v>
@@ -3927,20 +3927,20 @@
       <c r="CZ2" s="18"/>
       <c r="DA2" s="18"/>
       <c r="DB2" s="21" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="DJ2" s="21"/>
     </row>
     <row r="3" spans="1:114" s="23" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>165</v>
@@ -3950,16 +3950,16 @@
         <v>166</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="I3" s="24" t="s">
         <v>167</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="L3" s="25" t="s">
         <v>168</v>
@@ -4139,467 +4139,467 @@
         <v>226</v>
       </c>
       <c r="BS3" s="24" t="s">
-        <v>227</v>
+        <v>821</v>
       </c>
       <c r="BT3" s="24"/>
       <c r="BU3" s="24" t="s">
+        <v>822</v>
+      </c>
+      <c r="BV3" s="24" t="s">
+        <v>823</v>
+      </c>
+      <c r="BW3" s="24" t="s">
+        <v>824</v>
+      </c>
+      <c r="BX3" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="BY3" s="24" t="s">
+        <v>825</v>
+      </c>
+      <c r="BZ3" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="BV3" s="24" t="s">
+      <c r="CA3" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="BW3" s="24" t="s">
+      <c r="CB3" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="BX3" s="24" t="s">
+      <c r="CC3" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="BY3" s="24" t="s">
-        <v>655</v>
-      </c>
-      <c r="BZ3" s="25" t="s">
+      <c r="CD3" s="25" t="s">
+        <v>436</v>
+      </c>
+      <c r="CE3" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="CA3" s="24" t="s">
+      <c r="CF3" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="CB3" s="25" t="s">
+      <c r="CG3" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="CC3" s="24" t="s">
+      <c r="CH3" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="CD3" s="25" t="s">
-        <v>440</v>
-      </c>
-      <c r="CE3" s="24" t="s">
+      <c r="CI3" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="CF3" s="24" t="s">
+      <c r="CJ3" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="CG3" s="24" t="s">
+      <c r="CK3" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="CH3" s="24" t="s">
+      <c r="CL3" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="CM3" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="CN3" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="CP3" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="CI3" s="24" t="s">
+      <c r="CQ3" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="CJ3" s="24" t="s">
+      <c r="CR3" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="CK3" s="24" t="s">
+      <c r="CS3" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="CL3" s="24" t="s">
-        <v>401</v>
-      </c>
-      <c r="CM3" s="24" t="s">
-        <v>402</v>
-      </c>
-      <c r="CN3" s="24" t="s">
-        <v>403</v>
-      </c>
-      <c r="CP3" s="25" t="s">
+      <c r="CT3" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="CQ3" s="24" t="s">
+      <c r="CU3" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="CR3" s="24" t="s">
+      <c r="CV3" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="CS3" s="24" t="s">
+      <c r="CW3" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="CT3" s="24" t="s">
+      <c r="CX3" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="CU3" s="24" t="s">
+      <c r="CY3" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="CV3" s="25" t="s">
+      <c r="CZ3" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="CW3" s="24" t="s">
+      <c r="DA3" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="CX3" s="24" t="s">
-        <v>251</v>
-      </c>
-      <c r="CY3" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="CZ3" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="DA3" s="24" t="s">
-        <v>254</v>
-      </c>
       <c r="DB3" s="25" t="s">
+        <v>619</v>
+      </c>
+      <c r="DC3" s="24" t="s">
+        <v>620</v>
+      </c>
+      <c r="DD3" s="24" t="s">
+        <v>621</v>
+      </c>
+      <c r="DE3" s="24" t="s">
+        <v>622</v>
+      </c>
+      <c r="DF3" s="24" t="s">
         <v>623</v>
       </c>
-      <c r="DC3" s="24" t="s">
+      <c r="DG3" s="24" t="s">
         <v>624</v>
       </c>
-      <c r="DD3" s="24" t="s">
+      <c r="DH3" s="24" t="s">
         <v>625</v>
       </c>
-      <c r="DE3" s="24" t="s">
+      <c r="DI3" s="24" t="s">
         <v>626</v>
-      </c>
-      <c r="DF3" s="24" t="s">
-        <v>627</v>
-      </c>
-      <c r="DG3" s="24" t="s">
-        <v>628</v>
-      </c>
-      <c r="DH3" s="24" t="s">
-        <v>629</v>
-      </c>
-      <c r="DI3" s="24" t="s">
-        <v>630</v>
       </c>
       <c r="DJ3" s="26"/>
     </row>
     <row r="4" spans="1:114" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="H4" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="J4" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="L4" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>516</v>
-      </c>
-      <c r="I4" s="15" t="s">
+      <c r="M4" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="N4" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="O4" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="P4" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="Q4" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="R4" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="S4" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="T4" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="U4" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="R4" s="16" t="s">
+      <c r="V4" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="S4" s="15" t="s">
+      <c r="W4" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="X4" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="U4" s="15" t="s">
+      <c r="Y4" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="Z4" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="W4" s="15" t="s">
+      <c r="AA4" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="X4" s="16" t="s">
+      <c r="AB4" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="Y4" s="15" t="s">
+      <c r="AC4" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="Z4" s="15" t="s">
+      <c r="AD4" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="AA4" s="15" t="s">
+      <c r="AE4" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="AB4" s="15" t="s">
+      <c r="AF4" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="AC4" s="15" t="s">
+      <c r="AG4" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="AD4" s="15" t="s">
+      <c r="AH4" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="AE4" s="15" t="s">
+      <c r="AI4" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="AF4" s="16" t="s">
+      <c r="AJ4" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="AG4" s="15" t="s">
+      <c r="AK4" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="AH4" s="15" t="s">
+      <c r="AL4" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="AI4" s="15" t="s">
+      <c r="AM4" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="AJ4" s="16" t="s">
+      <c r="AN4" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="AK4" s="15" t="s">
+      <c r="AO4" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="AL4" s="15" t="s">
+      <c r="AP4" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="AM4" s="15" t="s">
+      <c r="AQ4" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="AN4" s="15" t="s">
+      <c r="AR4" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="AO4" s="15" t="s">
+      <c r="AS4" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="AP4" s="16" t="s">
+      <c r="AT4" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="AQ4" s="15" t="s">
+      <c r="AU4" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="AR4" s="15" t="s">
+      <c r="AV4" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="AS4" s="15" t="s">
+      <c r="AW4" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="AT4" s="15" t="s">
+      <c r="AX4" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="AU4" s="15" t="s">
+      <c r="AY4" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="AV4" s="15" t="s">
+      <c r="AZ4" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="AW4" s="15" t="s">
+      <c r="BA4" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="AX4" s="15" t="s">
+      <c r="BB4" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="AY4" s="15" t="s">
+      <c r="BC4" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="AZ4" s="15" t="s">
+      <c r="BD4" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="BA4" s="15" t="s">
+      <c r="BE4" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="BB4" s="15" t="s">
+      <c r="BF4" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="BC4" s="15" t="s">
+      <c r="BG4" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="BD4" s="16" t="s">
+      <c r="BH4" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="BE4" s="15" t="s">
+      <c r="BI4" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="BF4" s="16" t="s">
+      <c r="BJ4" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="BG4" s="15" t="s">
+      <c r="BK4" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="BH4" s="15" t="s">
+      <c r="BL4" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="BI4" s="15" t="s">
+      <c r="BM4" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="BJ4" s="15" t="s">
+      <c r="BN4" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="BK4" s="15" t="s">
+      <c r="BO4" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="BL4" s="15" t="s">
+      <c r="BP4" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="BM4" s="15" t="s">
+      <c r="BQ4" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="BN4" s="15" t="s">
+      <c r="BR4" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="BO4" s="15" t="s">
+      <c r="BS4" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="BP4" s="16" t="s">
+      <c r="BT4" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="BQ4" s="15" t="s">
+      <c r="BU4" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="BR4" s="16" t="s">
+      <c r="BV4" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="BS4" s="15" t="s">
+      <c r="BW4" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="BT4" s="15" t="s">
+      <c r="BX4" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="BU4" s="15" t="s">
+      <c r="BY4" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="BV4" s="15" t="s">
+      <c r="BZ4" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="BW4" s="15" t="s">
+      <c r="CA4" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="BX4" s="15" t="s">
+      <c r="CB4" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="BY4" s="15" t="s">
+      <c r="CC4" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="BZ4" s="16" t="s">
+      <c r="CD4" s="16" t="s">
+        <v>795</v>
+      </c>
+      <c r="CE4" s="15" t="s">
+        <v>796</v>
+      </c>
+      <c r="CF4" s="15" t="s">
+        <v>797</v>
+      </c>
+      <c r="CG4" s="15" t="s">
+        <v>798</v>
+      </c>
+      <c r="CH4" s="15" t="s">
+        <v>799</v>
+      </c>
+      <c r="CI4" s="15" t="s">
+        <v>800</v>
+      </c>
+      <c r="CJ4" s="15" t="s">
+        <v>801</v>
+      </c>
+      <c r="CK4" s="15" t="s">
+        <v>802</v>
+      </c>
+      <c r="CL4" s="15" t="s">
+        <v>803</v>
+      </c>
+      <c r="CM4" s="15" t="s">
+        <v>804</v>
+      </c>
+      <c r="CN4" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="CP4" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="CA4" s="15" t="s">
+      <c r="CQ4" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="CB4" s="16" t="s">
+      <c r="CR4" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="CC4" s="15" t="s">
+      <c r="CS4" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="CD4" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="CE4" s="15" t="s">
-        <v>801</v>
-      </c>
-      <c r="CF4" s="15" t="s">
-        <v>802</v>
-      </c>
-      <c r="CG4" s="15" t="s">
-        <v>803</v>
-      </c>
-      <c r="CH4" s="15" t="s">
-        <v>804</v>
-      </c>
-      <c r="CI4" s="15" t="s">
-        <v>805</v>
-      </c>
-      <c r="CJ4" s="15" t="s">
-        <v>806</v>
-      </c>
-      <c r="CK4" s="15" t="s">
-        <v>807</v>
-      </c>
-      <c r="CL4" s="15" t="s">
-        <v>808</v>
-      </c>
-      <c r="CM4" s="15" t="s">
-        <v>809</v>
-      </c>
-      <c r="CN4" s="9" t="s">
-        <v>810</v>
-      </c>
-      <c r="CP4" s="16" t="s">
+      <c r="CT4" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="CQ4" s="15" t="s">
+      <c r="CU4" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="CR4" s="15" t="s">
+      <c r="CV4" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="CS4" s="15" t="s">
+      <c r="CW4" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="CT4" s="15" t="s">
+      <c r="CX4" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="CU4" s="15" t="s">
+      <c r="CY4" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="CV4" s="16" t="s">
+      <c r="CZ4" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="CW4" s="15" t="s">
+      <c r="DA4" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="CX4" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="CY4" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="CZ4" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="DA4" s="15" t="s">
-        <v>346</v>
-      </c>
       <c r="DB4" s="21" t="s">
+        <v>627</v>
+      </c>
+      <c r="DC4" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="DD4" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="DE4" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="DF4" s="17" t="s">
         <v>631</v>
       </c>
-      <c r="DC4" s="9" t="s">
+      <c r="DG4" s="9" t="s">
         <v>632</v>
       </c>
-      <c r="DD4" s="9" t="s">
+      <c r="DH4" s="9" t="s">
         <v>633</v>
       </c>
-      <c r="DE4" s="9" t="s">
+      <c r="DI4" s="9" t="s">
         <v>634</v>
-      </c>
-      <c r="DF4" s="17" t="s">
-        <v>635</v>
-      </c>
-      <c r="DG4" s="9" t="s">
-        <v>636</v>
-      </c>
-      <c r="DH4" s="9" t="s">
-        <v>637</v>
-      </c>
-      <c r="DI4" s="9" t="s">
-        <v>638</v>
       </c>
       <c r="DJ4" s="21"/>
     </row>
@@ -4980,7 +4980,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="22" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4988,64 +4988,64 @@
         <v>21</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>600</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>604</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>606</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>607</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>608</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>609</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>610</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>611</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:10" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>617</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>618</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>619</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>620</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -5070,157 +5070,157 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="22" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B3" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C3" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D3" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="E3" t="s">
+        <v>477</v>
+      </c>
+      <c r="F3" t="s">
+        <v>478</v>
+      </c>
+      <c r="G3" t="s">
+        <v>479</v>
+      </c>
+      <c r="H3" t="s">
+        <v>480</v>
+      </c>
+      <c r="I3" t="s">
         <v>481</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>482</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>483</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>484</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>486</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>487</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>488</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>489</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
         <v>490</v>
       </c>
-      <c r="O3" t="s">
+      <c r="S3" t="s">
         <v>491</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" t="s">
         <v>492</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="U3" t="s">
         <v>493</v>
       </c>
-      <c r="R3" t="s">
+      <c r="V3" t="s">
         <v>494</v>
-      </c>
-      <c r="S3" t="s">
-        <v>495</v>
-      </c>
-      <c r="T3" t="s">
-        <v>496</v>
-      </c>
-      <c r="U3" t="s">
-        <v>497</v>
-      </c>
-      <c r="V3" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="D4" s="12" t="s">
+        <v>806</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>464</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>811</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>462</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>461</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="M4" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="Q4" s="12" t="s">
         <v>467</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>470</v>
-      </c>
-      <c r="M4" s="12" t="s">
+      <c r="R4" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="U4" s="12" t="s">
         <v>475</v>
       </c>
-      <c r="N4" s="12" t="s">
-        <v>474</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>473</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>472</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>471</v>
-      </c>
-      <c r="R4" s="12" t="s">
+      <c r="V4" s="12" t="s">
         <v>476</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>477</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>478</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>479</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -5278,49 +5278,49 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="22" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>734</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>739</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>743</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B3" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C3" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D3" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -5348,44 +5348,44 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="22" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" t="s">
         <v>438</v>
       </c>
-      <c r="B3" t="s">
-        <v>442</v>
-      </c>
       <c r="C3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E3" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F3" t="s">
         <v>84</v>
@@ -5393,22 +5393,22 @@
     </row>
     <row r="4" spans="1:6" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>447</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>448</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>450</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -5520,16 +5520,16 @@
         <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>57</v>
       </c>
       <c r="N1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -5572,7 +5572,7 @@
         <v>67</v>
       </c>
       <c r="Q3" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -5595,7 +5595,7 @@
         <v>68</v>
       </c>
       <c r="Q4" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>69</v>
       </c>
       <c r="Q5" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -5629,7 +5629,7 @@
         <v>70</v>
       </c>
       <c r="Q6" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -5646,7 +5646,7 @@
         <v>71</v>
       </c>
       <c r="Q7" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -5663,7 +5663,7 @@
         <v>72</v>
       </c>
       <c r="Q8" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
@@ -5680,7 +5680,7 @@
         <v>73</v>
       </c>
       <c r="Q9" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -5697,7 +5697,7 @@
         <v>74</v>
       </c>
       <c r="Q10" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -5837,103 +5837,103 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="I2" s="22" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B3" t="s">
+        <v>514</v>
+      </c>
+      <c r="C3" t="s">
+        <v>515</v>
+      </c>
+      <c r="D3" t="s">
+        <v>516</v>
+      </c>
+      <c r="E3" t="s">
         <v>517</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>518</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>519</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>520</v>
-      </c>
-      <c r="E3" t="s">
-        <v>521</v>
-      </c>
-      <c r="F3" t="s">
-        <v>522</v>
-      </c>
-      <c r="G3" t="s">
-        <v>523</v>
-      </c>
-      <c r="H3" t="s">
-        <v>524</v>
       </c>
       <c r="I3" t="s">
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>530</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>531</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>533</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5973,48 +5973,48 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>667</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>669</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>755</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>671</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>672</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>673</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>674</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>675</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>760</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>677</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>678</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>679</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>680</v>
-      </c>
       <c r="L2" s="22" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -6022,7 +6022,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C3" t="s">
         <v>102</v>
@@ -6046,7 +6046,7 @@
         <v>35</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>127</v>
@@ -6060,43 +6060,43 @@
     </row>
     <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>355</v>
-      </c>
       <c r="J4" s="9" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="P4" s="9"/>
     </row>
@@ -6160,54 +6160,54 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="22" customFormat="1" ht="189.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
+        <v>655</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>745</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>746</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>747</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>748</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>749</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>750</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>659</v>
+      </c>
+      <c r="N2" s="22" t="s">
         <v>660</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="O2" s="22" t="s">
         <v>661</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>749</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>750</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>751</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>752</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>753</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>663</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>754</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>755</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>756</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>664</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>665</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="48" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6224,13 +6224,13 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="F3" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="H3" t="s">
         <v>24</v>
@@ -6262,49 +6262,49 @@
     </row>
     <row r="4" spans="1:18" s="9" customFormat="1" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="L4" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>364</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6374,30 +6374,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -6425,25 +6425,25 @@
     </row>
     <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>371</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6508,54 +6508,54 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>501</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>504</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>502</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>503</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>505</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>508</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>510</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>511</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -6586,66 +6586,66 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>759</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>760</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>678</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>761</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>679</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>762</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>681</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>763</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>682</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>684</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>685</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>686</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>764</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>765</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>766</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>684</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>767</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>686</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>768</v>
-      </c>
-      <c r="J2" s="22" t="s">
+      <c r="P2" s="22" t="s">
+        <v>690</v>
+      </c>
+      <c r="Q2" s="22" t="s">
         <v>687</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="R2" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="S2" s="22" t="s">
         <v>689</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>690</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>769</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>695</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>692</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>693</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -6718,61 +6718,61 @@
     </row>
     <row r="4" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>393</v>
-      </c>
       <c r="S4" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -6827,121 +6827,121 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="22" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>765</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>766</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>767</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>768</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>769</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>770</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>771</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>772</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>773</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>774</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>775</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>776</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>777</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="78.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>651</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>108</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>571</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>572</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="F4" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>576</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>575</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>574</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>573</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>578</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>579</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>580</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>581</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -6976,54 +6976,54 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="22" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>691</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>774</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>775</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>693</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>694</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>695</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>696</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>697</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>696</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>779</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>780</v>
-      </c>
-      <c r="F2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>698</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>699</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="M2" s="22" t="s">
         <v>700</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="N2" s="22" t="s">
         <v>701</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="O2" s="22" t="s">
         <v>702</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>703</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>704</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>705</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>706</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -7070,54 +7070,54 @@
         <v>124</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="13" customFormat="1" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="G4" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>405</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="J4" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="K4" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="L4" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="M4" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="N4" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="K4" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>416</v>
-      </c>
       <c r="O4" s="13" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Allow reference to external file for instance
Allow reference to external file instead of only to dataset for instance
</commit_message>
<xml_diff>
--- a/excel_template.xlsx
+++ b/excel_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\for_PDB\excel2mmcif\20191031_excel2mmcif_addition_of_lifetime_based_analysis\20191106_preparation_of_T4L_files\raw_files_for_excel2mmcif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\excel2mmcif_working_directory\tmp_directory_for_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="730" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="19" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="943">
   <si>
     <t>Model number</t>
   </si>
@@ -2896,6 +2896,15 @@
   </si>
   <si>
     <t>IHM_Dataset_top_directory</t>
+  </si>
+  <si>
+    <t>The external file ID (Tab 'External_files') if available</t>
+  </si>
+  <si>
+    <t>starting model external file id</t>
+  </si>
+  <si>
+    <t>IHM_Instance_Starting_model_external_file_id</t>
   </si>
 </sst>
 </file>
@@ -3714,7 +3723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -32418,9 +32427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33275,8 +33282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -33350,6 +33357,9 @@
       <c r="S2" s="20" t="s">
         <v>687</v>
       </c>
+      <c r="T2" s="76" t="s">
+        <v>940</v>
+      </c>
     </row>
     <row r="3" spans="1:28" ht="63" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -33409,7 +33419,9 @@
       <c r="S3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="T3" s="1"/>
+      <c r="T3" s="1" t="s">
+        <v>941</v>
+      </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
@@ -33477,6 +33489,9 @@
       <c r="S4" s="7" t="s">
         <v>393</v>
       </c>
+      <c r="T4" s="71" t="s">
+        <v>942</v>
+      </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D5" s="67"/>
@@ -33528,7 +33543,7 @@
       <c r="B13" s="66"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P1048576">
       <formula1>"comparative model, experimental model, integrative model, ab initio model, other"</formula1>
     </dataValidation>
@@ -33546,6 +33561,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1048576">
       <formula1>entity_id</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T1048576">
+      <formula1>external_file_id</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix some missing selection for some rows in "Dataset"
</commit_message>
<xml_diff>
--- a/excel_template.xlsx
+++ b/excel_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336" tabRatio="730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336" tabRatio="730" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="19" r:id="rId1"/>
@@ -3784,7 +3784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -32604,8 +32604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -32923,8 +32923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -33113,8 +33113,11 @@
       <c r="Q5" s="82"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R6" s="2"/>
+    <row r="6" spans="1:21" s="65" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N6" s="8"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="66"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F7" s="1"/>
@@ -33123,16 +33126,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7:L1048576 L5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L1048576">
       <formula1>"Zenodo, Figshare, Crossref"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7:M1048576 M5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M1048576">
       <formula1>"DOI, Supplementary Files"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1048576 O5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576">
       <formula1>"File, Archive, Publication, Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G1048576 G5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1048576">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -33145,13 +33148,13 @@
           <x14:formula1>
             <xm:f>for_internal_use_only!$K$3:$K$22</xm:f>
           </x14:formula1>
-          <xm:sqref>F7:F1048576 F5</xm:sqref>
+          <xm:sqref>F5:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>for_internal_use_only!$L$3:$L$14</xm:f>
           </x14:formula1>
-          <xm:sqref>H5 H8:H1048576</xm:sqref>
+          <xm:sqref>H5:H6 H8:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>